<commit_message>
Ported C code over for filtering Data_Processing
works somewhat, still might need tweaking
</commit_message>
<xml_diff>
--- a/Matlab/CppFriendlyCode/testdata.xlsx
+++ b/Matlab/CppFriendlyCode/testdata.xlsx
@@ -28,7 +28,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -62,11 +62,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -94,6 +95,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>

<commit_message>
Matlab changes for isolating PTT function
</commit_message>
<xml_diff>
--- a/Matlab/CppFriendlyCode/testdata.xlsx
+++ b/Matlab/CppFriendlyCode/testdata.xlsx
@@ -28,7 +28,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -63,11 +63,25 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -96,6 +110,20 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>